<commit_message>
Developed new Methods and updated Timeouts
</commit_message>
<xml_diff>
--- a/src/test/resources/datasheets/AddInternalComments.xlsx
+++ b/src/test/resources/datasheets/AddInternalComments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15045" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="Verify_AddInternalComments" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -48,10 +49,10 @@
     <t>Item Added Successfully</t>
   </si>
   <si>
-    <t>Cell Phones</t>
-  </si>
-  <si>
     <t>EA-EACH</t>
+  </si>
+  <si>
+    <t>Computers</t>
   </si>
 </sst>
 </file>
@@ -386,7 +387,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -425,10 +426,10 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
       <c r="F2">
         <v>1</v>

</xml_diff>